<commit_message>
Update Gantt Chart for Project Plan.md
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisky\Documents\Repositories\Griffith\2810ICT-milestone-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC270A7-1D57-4B62-8AAE-BDE25FD8137F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB61950C-02B0-4788-AC86-819A40716A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5235" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -673,6 +673,33 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -684,33 +711,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1114,8 +1114,8 @@
   </sheetPr>
   <dimension ref="B1:BE48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="30" customHeight="1" outlineLevelRow="2"/>
@@ -1146,11 +1146,11 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:57" ht="33.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="G2" s="21" t="s">
         <v>11</v>
       </c>
@@ -1158,37 +1158,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="29"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="31" t="s">
+      <c r="Q2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="33"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="29"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="37"/>
+      <c r="V2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="33"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AA2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="33"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
         <v>3</v>
@@ -1202,22 +1202,22 @@
       <c r="AP2" s="20"/>
     </row>
     <row r="3" spans="2:57" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="25" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1244,12 +1244,12 @@
       <c r="AA3" s="8"/>
     </row>
     <row r="4" spans="2:57" ht="15.75" customHeight="1">
-      <c r="B4" s="27"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1854,9 +1854,11 @@
       <c r="E27" s="5">
         <v>24</v>
       </c>
-      <c r="F27" s="5"/>
+      <c r="F27" s="5">
+        <v>14</v>
+      </c>
       <c r="G27" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="31.5" outlineLevel="1">
@@ -2186,17 +2188,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BE4">
     <cfRule type="expression" dxfId="8" priority="8">

</xml_diff>